<commit_message>
Adjust SHACL and XSL for proper SHACL validation of ORG Dataset
</commit_message>
<xml_diff>
--- a/Subtask5/01-cv/04-SHACL/CV-Shapes.xlsx
+++ b/Subtask5/01-cv/04-SHACL/CV-Shapes.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="172">
   <si>
     <t xml:space="preserve">Shapes URI</t>
   </si>
@@ -392,7 +392,7 @@
     <t xml:space="preserve">rdf:langString</t>
   </si>
   <si>
-    <t xml:space="preserve">("da" "de" "en" "es" "fr" "it" "nl" "el" "sv" "fi" "cs" "et" "lt" "hu" "mt" "pl" "sk" "sl" "ro" "bg" "ga" "lv" "hr")</t>
+    <t xml:space="preserve">("da" "de" "en" "es" "fr" "it" "nl" "el" "sv" "fi" "cs" "et" "lt" "hu" "mt" "pl" "pt" "sk" "sl" "ro" "bg" "ga" "lv" "hr")</t>
   </si>
   <si>
     <t xml:space="preserve">skos:prefLabel</t>
@@ -458,7 +458,7 @@
     <t xml:space="preserve">[A-Z][A-Z]</t>
   </si>
   <si>
-    <t xml:space="preserve">eponto:isoNumber</t>
+    <t xml:space="preserve">org-ep:isoNumber</t>
   </si>
   <si>
     <t xml:space="preserve">ISO number</t>
@@ -521,19 +521,10 @@
     <t xml:space="preserve">ep-aut:parliamentary-term</t>
   </si>
   <si>
-    <t xml:space="preserve">Iso Language</t>
-  </si>
-  <si>
-    <t xml:space="preserve">org-ep:Period</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Period</t>
-  </si>
-  <si>
     <t xml:space="preserve">dct:temporal</t>
   </si>
   <si>
-    <t xml:space="preserve">Temporal</t>
+    <t xml:space="preserve">temporal</t>
   </si>
   <si>
     <t xml:space="preserve">(skos:Concept org-ep:parliamentary-term)</t>
@@ -556,7 +547,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -630,13 +621,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <strike val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -701,7 +685,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -786,14 +770,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -874,11 +850,11 @@
   </sheetPr>
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I17" activeCellId="0" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.515625" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.59"/>
@@ -1311,13 +1287,13 @@
   </sheetPr>
   <dimension ref="A1:U1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="9" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="9" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
+      <selection pane="bottomLeft" activeCell="T33" activeCellId="0" sqref="T33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.99"/>
@@ -1335,8 +1311,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="34.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="28.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="21.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="28.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="21.56"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1651,7 +1627,7 @@
       </c>
       <c r="R13" s="13"/>
     </row>
-    <row r="14" customFormat="false" ht="37.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="str">
         <f aca="false">CONCATENATE("epsh:P",ROW(A14))</f>
         <v>epsh:P14</v>
@@ -1678,7 +1654,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="37.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="str">
         <f aca="false">CONCATENATE("epsh:P",ROW(A15))</f>
         <v>epsh:P15</v>
@@ -2071,37 +2047,37 @@
         <v>117</v>
       </c>
     </row>
-    <row r="31" s="21" customFormat="true" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="21" t="str">
+    <row r="31" s="20" customFormat="true" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="20" t="str">
         <f aca="false">CONCATENATE("epsh:P",ROW(A31))</f>
         <v>epsh:P31</v>
       </c>
-      <c r="B31" s="21" t="s">
+      <c r="B31" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="C31" s="22" t="s">
+      <c r="C31" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="D31" s="22" t="n">
+      <c r="D31" s="14" t="n">
         <v>6</v>
       </c>
-      <c r="E31" s="21" t="s">
+      <c r="E31" s="20" t="s">
         <v>146</v>
       </c>
-      <c r="F31" s="22"/>
-      <c r="G31" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="H31" s="21" t="n">
-        <v>1</v>
-      </c>
-      <c r="L31" s="21" t="s">
+      <c r="F31" s="14"/>
+      <c r="G31" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="H31" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="L31" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="M31" s="21" t="s">
+      <c r="M31" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="T31" s="22"/>
+      <c r="T31" s="14"/>
     </row>
     <row r="32" customFormat="false" ht="37.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="str">
@@ -2142,7 +2118,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="37.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="str">
         <f aca="false">CONCATENATE("epsh:P",ROW(A33))</f>
         <v>epsh:P33</v>
@@ -2158,15 +2134,6 @@
       </c>
       <c r="E33" s="0" t="s">
         <v>121</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="G33" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="H33" s="0" t="n">
-        <v>24</v>
       </c>
       <c r="L33" s="0" t="s">
         <v>116</v>
@@ -2359,7 +2326,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="37.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="69.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="str">
         <f aca="false">CONCATENATE("epsh:P",ROW(A42))</f>
         <v>epsh:P42</v>
@@ -2551,7 +2518,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="37.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="58.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="str">
         <f aca="false">CONCATENATE("epsh:P",ROW(A51))</f>
         <v>epsh:P51</v>
@@ -2647,13 +2614,13 @@
         <v>165</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="str">
         <f aca="false">CONCATENATE("epsh:P",ROW(A57))</f>
         <v>epsh:P57</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>9</v>
+        <v>124</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>61</v>
@@ -2662,7 +2629,7 @@
         <v>2</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>153</v>
+        <v>125</v>
       </c>
       <c r="G57" s="1" t="n">
         <v>1</v>
@@ -2674,7 +2641,7 @@
         <v>116</v>
       </c>
       <c r="M57" s="0" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2683,16 +2650,16 @@
         <v>epsh:P58</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>114</v>
+        <v>166</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>61</v>
       </c>
       <c r="D58" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="G58" s="1" t="n">
         <v>1</v>
@@ -2707,120 +2674,118 @@
         <v>117</v>
       </c>
     </row>
-    <row r="59" s="21" customFormat="true" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="21" t="str">
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="str">
         <f aca="false">CONCATENATE("epsh:P",ROW(A59))</f>
         <v>epsh:P59</v>
       </c>
-      <c r="B59" s="21" t="s">
-        <v>167</v>
-      </c>
-      <c r="C59" s="22" t="s">
+      <c r="B59" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="C59" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D59" s="22" t="n">
-        <v>4</v>
-      </c>
-      <c r="E59" s="21" t="s">
-        <v>168</v>
-      </c>
-      <c r="F59" s="22"/>
-      <c r="G59" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="H59" s="21" t="n">
-        <v>1</v>
-      </c>
-      <c r="L59" s="21" t="s">
+      <c r="D59" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="E59" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="G59" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H59" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L59" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="M59" s="21" t="s">
+      <c r="M59" s="0" t="s">
         <v>117</v>
       </c>
-      <c r="T59" s="22"/>
-    </row>
-    <row r="60" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="60" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="str">
         <f aca="false">CONCATENATE("epsh:P",ROW(A60))</f>
         <v>epsh:P60</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>169</v>
+        <v>7</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>61</v>
       </c>
       <c r="D60" s="1" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E60" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G60" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="H60" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q60" s="0" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="63" s="18" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A63" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="T63" s="19"/>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="str">
+        <f aca="false">CONCATENATE("epsh:P",ROW(A64))</f>
+        <v>epsh:P64</v>
+      </c>
+      <c r="B64" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D64" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="G64" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H64" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L64" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="U64" s="0" t="s">
         <v>170</v>
       </c>
-      <c r="G60" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="H60" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="L60" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="M60" s="0" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="37.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="str">
-        <f aca="false">CONCATENATE("epsh:P",ROW(A61))</f>
-        <v>epsh:P61</v>
-      </c>
-      <c r="B61" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D61" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="E61" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="G61" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="H61" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q61" s="0" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="64" s="18" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A64" s="18" t="s">
-        <v>172</v>
-      </c>
-      <c r="T64" s="19"/>
-    </row>
-    <row r="65" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="65" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="str">
         <f aca="false">CONCATENATE("epsh:P",ROW(A65))</f>
         <v>epsh:P65</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>111</v>
+        <v>133</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>65</v>
       </c>
       <c r="D65" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>112</v>
+        <v>134</v>
       </c>
       <c r="G65" s="1" t="n">
         <v>1</v>
@@ -2829,40 +2794,37 @@
         <v>1</v>
       </c>
       <c r="L65" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="U65" s="0" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>116</v>
+      </c>
+      <c r="M65" s="0" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="55.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="str">
         <f aca="false">CONCATENATE("epsh:P",ROW(A66))</f>
         <v>epsh:P66</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>9</v>
+        <v>124</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>65</v>
       </c>
       <c r="D66" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>153</v>
+        <v>125</v>
       </c>
       <c r="G66" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="H66" s="0" t="n">
         <v>1</v>
       </c>
       <c r="L66" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="M66" s="0" t="s">
-        <v>117</v>
+      <c r="S66" s="0" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="37.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2871,66 +2833,31 @@
         <v>epsh:P67</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>124</v>
+        <v>7</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>65</v>
       </c>
       <c r="D67" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>127</v>
       </c>
       <c r="G67" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H67" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="L67" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="M67" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="S67" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="T67" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="37.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="str">
-        <f aca="false">CONCATENATE("epsh:P",ROW(A68))</f>
-        <v>epsh:P68</v>
-      </c>
-      <c r="B68" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D68" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E68" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="F68" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="G68" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="H68" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q68" s="0" t="s">
-        <v>174</v>
-      </c>
-    </row>
+      <c r="Q67" s="0" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>